<commit_message>
final edits to DoCalculations.py
</commit_message>
<xml_diff>
--- a/results/resultsDwg.xlsx
+++ b/results/resultsDwg.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -429,13 +429,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>24.12606812724482</v>
+        <v>5.499559799734492</v>
       </c>
       <c r="F2">
-        <v>43.01490000000003</v>
+        <v>110.3084</v>
       </c>
       <c r="G2">
-        <v>3.761546567300181</v>
+        <v>4.70328007929809</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -452,13 +452,13 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>11.96941394602459</v>
+        <v>4.862806372923105</v>
       </c>
       <c r="F3">
-        <v>197.7015</v>
+        <v>182.3177</v>
       </c>
       <c r="G3">
-        <v>5.286758317401202</v>
+        <v>5.20575076967576</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -475,13 +475,13 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>32.56436843238451</v>
+        <v>7.208790910217862</v>
       </c>
       <c r="F4">
-        <v>54.8809</v>
+        <v>179.2462</v>
       </c>
       <c r="G4">
-        <v>4.005165382700071</v>
+        <v>5.188760279812898</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -498,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>19.70534279157461</v>
+        <v>6.738687873765687</v>
       </c>
       <c r="F5">
         <v>153.4924</v>
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -521,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>38.36752202498447</v>
+        <v>15.37566223470216</v>
       </c>
       <c r="F6">
         <v>49.6541</v>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -544,13 +544,13 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>23.97110304753747</v>
+        <v>9.267816989804006</v>
       </c>
       <c r="F7">
-        <v>93.31489999999999</v>
+        <v>83.9725</v>
       </c>
       <c r="G7">
-        <v>4.535979794995447</v>
+        <v>4.430489364290089</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -567,7 +567,7 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>18.46432834330068</v>
+        <v>5.952741952558664</v>
       </c>
       <c r="F8">
         <v>96.15370000000001</v>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <v>7.72367965601982</v>
+        <v>2.387551295565076</v>
       </c>
       <c r="F9">
         <v>48.5907</v>
@@ -604,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -613,7 +613,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>16.56123730111453</v>
+        <v>7.581392153200484</v>
       </c>
       <c r="F10">
         <v>45.8028</v>
@@ -627,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>40.45823380334502</v>
+        <v>13.14521693838559</v>
       </c>
       <c r="F11">
         <v>41.0215</v>
@@ -650,7 +650,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>25.14864932089196</v>
+        <v>10.21325955490269</v>
       </c>
       <c r="F12">
         <v>117.9755</v>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>16.25213823881749</v>
+        <v>5.888714435624997</v>
       </c>
       <c r="F13">
         <v>309.8063999999999</v>
@@ -696,7 +696,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -705,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>17.66855273985791</v>
+        <v>6.289615094785585</v>
       </c>
       <c r="F14">
         <v>341.0163</v>
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="E15">
-        <v>14.37764443870789</v>
+        <v>5.626986961249971</v>
       </c>
       <c r="F15">
         <v>102.4596</v>
@@ -742,7 +742,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -751,7 +751,7 @@
         <v>5</v>
       </c>
       <c r="E16">
-        <v>36.63688813508279</v>
+        <v>14.02275603607696</v>
       </c>
       <c r="F16">
         <v>124.9963</v>
@@ -765,7 +765,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -774,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="E17">
-        <v>22.99674957280322</v>
+        <v>10.0576511745145</v>
       </c>
       <c r="F17">
-        <v>47.146</v>
+        <v>39.147</v>
       </c>
       <c r="G17">
-        <v>3.853249169849756</v>
+        <v>3.667323791148219</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -788,7 +788,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -797,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>16.72449723887421</v>
+        <v>5.45206934187958</v>
       </c>
       <c r="F18">
         <v>162.7357</v>
@@ -811,7 +811,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -820,13 +820,13 @@
         <v>8</v>
       </c>
       <c r="E19">
-        <v>15.21119781213687</v>
+        <v>4.504491233455119</v>
       </c>
       <c r="F19">
-        <v>128.8005</v>
+        <v>125.4816</v>
       </c>
       <c r="G19">
-        <v>4.858264695650296</v>
+        <v>4.832159134277205</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -834,7 +834,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="E20">
-        <v>22.77302391247592</v>
+        <v>10.71997967712378</v>
       </c>
       <c r="F20">
         <v>58.4853</v>
@@ -857,22 +857,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>25.06016463290939</v>
+        <v>12.01020739063222</v>
       </c>
       <c r="F21">
-        <v>60.15670000000001</v>
+        <v>30.4858</v>
       </c>
       <c r="G21">
-        <v>4.09695282441366</v>
+        <v>3.417261001429755</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -880,22 +880,22 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>16.09861693549157</v>
+        <v>8.69765092763909</v>
       </c>
       <c r="F22">
-        <v>108.3519</v>
+        <v>60.15670000000001</v>
       </c>
       <c r="G22">
-        <v>4.685384263592347</v>
+        <v>4.09695282441366</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -903,22 +903,22 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>22.99781721909175</v>
+        <v>6.845959030997408</v>
       </c>
       <c r="F23">
-        <v>96.68560000000001</v>
+        <v>108.3519</v>
       </c>
       <c r="G23">
-        <v>4.571464477202904</v>
+        <v>4.685384263592347</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -926,22 +926,22 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>19.22601501482956</v>
+        <v>8.072575184504698</v>
       </c>
       <c r="F24">
-        <v>65.61760000000001</v>
+        <v>96.68560000000001</v>
       </c>
       <c r="G24">
-        <v>4.183843952648925</v>
+        <v>4.571464477202904</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -949,22 +949,22 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>18.39538373723202</v>
+        <v>7.854056330729034</v>
       </c>
       <c r="F25">
-        <v>46.7971</v>
+        <v>65.61760000000001</v>
       </c>
       <c r="G25">
-        <v>3.845821235191675</v>
+        <v>4.183843952648925</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -972,22 +972,22 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>21.46070556203179</v>
+        <v>6.55175804511823</v>
       </c>
       <c r="F26">
-        <v>92.15310000000001</v>
+        <v>46.7971</v>
       </c>
       <c r="G26">
-        <v>4.523451324353032</v>
+        <v>3.845821235191675</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -995,22 +995,22 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>17.43726423090362</v>
+        <v>8.05657344684022</v>
       </c>
       <c r="F27">
-        <v>86.91</v>
+        <v>24.8924</v>
       </c>
       <c r="G27">
-        <v>4.464873100449369</v>
+        <v>3.214562535997754</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1018,22 +1018,22 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>11.67227794846325</v>
+        <v>7.508297925139551</v>
       </c>
       <c r="F28">
-        <v>42.4834</v>
+        <v>92.15310000000001</v>
       </c>
       <c r="G28">
-        <v>3.749113411395624</v>
+        <v>4.523451324353032</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1041,22 +1041,22 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E29">
-        <v>16.98002652176273</v>
+        <v>6.438437642880476</v>
       </c>
       <c r="F29">
-        <v>66.7795</v>
+        <v>86.91</v>
       </c>
       <c r="G29">
-        <v>4.20139614721584</v>
+        <v>4.464873100449369</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1064,22 +1064,22 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E30">
-        <v>7.49398852869661</v>
+        <v>5.477645474213253</v>
       </c>
       <c r="F30">
-        <v>78.44599999999998</v>
+        <v>42.4834</v>
       </c>
       <c r="G30">
-        <v>4.362410489988739</v>
+        <v>3.749113411395624</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1087,22 +1087,22 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E31">
-        <v>16.40806098059358</v>
+        <v>26.87253961095874</v>
       </c>
       <c r="F31">
-        <v>163.7829</v>
+        <v>18.5212</v>
       </c>
       <c r="G31">
-        <v>5.098541770364973</v>
+        <v>2.918916021935355</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1110,22 +1110,22 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>9.363513211474832</v>
+        <v>5.139864235504609</v>
       </c>
       <c r="F32">
-        <v>73.4663</v>
+        <v>45.40479999999999</v>
       </c>
       <c r="G32">
-        <v>4.296826797672606</v>
+        <v>3.815617826330857</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1133,22 +1133,22 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>17.94814829725615</v>
+        <v>4.22699721480902</v>
       </c>
       <c r="F33">
-        <v>145.4427</v>
+        <v>106.1594000000001</v>
       </c>
       <c r="G33">
-        <v>4.979782194613289</v>
+        <v>4.664941738161711</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1156,22 +1156,22 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>9.26420843180146</v>
+        <v>5.099697709902927</v>
       </c>
       <c r="F34">
-        <v>241.6773</v>
+        <v>168.9935</v>
       </c>
       <c r="G34">
-        <v>5.487603365218593</v>
+        <v>5.129860252644948</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1179,22 +1179,22 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>12.30272000430799</v>
+        <v>5.240186963098562</v>
       </c>
       <c r="F35">
-        <v>190.6974</v>
+        <v>39.87730000000001</v>
       </c>
       <c r="G35">
-        <v>5.250687878533356</v>
+        <v>3.685807239692351</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1202,22 +1202,22 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
         <v>5</v>
       </c>
-      <c r="D36">
-        <v>4</v>
-      </c>
       <c r="E36">
-        <v>13.98520508973004</v>
+        <v>6.941580343295782</v>
       </c>
       <c r="F36">
-        <v>77.63359999999999</v>
+        <v>73.28540000000001</v>
       </c>
       <c r="G36">
-        <v>4.352000323166909</v>
+        <v>4.294361407607235</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1225,22 +1225,22 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>8.510726257160156</v>
+        <v>3.104546112068172</v>
       </c>
       <c r="F37">
-        <v>76.83629999999999</v>
+        <v>9.973400000000002</v>
       </c>
       <c r="G37">
-        <v>4.341677184736846</v>
+        <v>2.299921548907804</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1248,22 +1248,22 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>7</v>
       </c>
       <c r="E38">
-        <v>15.9047173217216</v>
+        <v>6.163729553040468</v>
       </c>
       <c r="F38">
-        <v>129.7927</v>
+        <v>12.463</v>
       </c>
       <c r="G38">
-        <v>4.865938562318641</v>
+        <v>2.52276425484424</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1271,22 +1271,22 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D39">
         <v>8</v>
       </c>
       <c r="E39">
-        <v>12.85118222786222</v>
+        <v>5.724250436831811</v>
       </c>
       <c r="F39">
-        <v>191.5773</v>
+        <v>92.63590000000002</v>
       </c>
       <c r="G39">
-        <v>5.255291382526276</v>
+        <v>4.528676755505058</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1294,22 +1294,22 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C40">
         <v>5</v>
       </c>
       <c r="D40">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>23.27811679687173</v>
+        <v>7.335283268065345</v>
       </c>
       <c r="F40">
-        <v>72.887</v>
+        <v>30.751</v>
       </c>
       <c r="G40">
-        <v>4.288910296637933</v>
+        <v>3.425922514048956</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1317,22 +1317,22 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="E41">
-        <v>22.12037402002544</v>
+        <v>4.569044865771998</v>
       </c>
       <c r="F41">
-        <v>59.21180000000002</v>
+        <v>49.7358</v>
       </c>
       <c r="G41">
-        <v>4.081120846351831</v>
+        <v>3.906724995726846</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1340,22 +1340,22 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42">
-        <v>9.219863824493219</v>
+        <v>5.520305980587588</v>
       </c>
       <c r="F42">
-        <v>193.2362</v>
+        <v>48.34210000000002</v>
       </c>
       <c r="G42">
-        <v>5.263913274827154</v>
+        <v>3.878302816615572</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1363,22 +1363,22 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E43">
-        <v>10.12287619843626</v>
+        <v>3.884676391726787</v>
       </c>
       <c r="F43">
-        <v>91.35730000000002</v>
+        <v>53.85239999999999</v>
       </c>
       <c r="G43">
-        <v>4.514778192055928</v>
+        <v>3.986246970854388</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1386,22 +1386,22 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E44">
-        <v>24.70908350289245</v>
+        <v>4.742593543371395</v>
       </c>
       <c r="F44">
-        <v>53.4702</v>
+        <v>60.85520000000001</v>
       </c>
       <c r="G44">
-        <v>3.979124489368831</v>
+        <v>4.108497271821818</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1409,22 +1409,22 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
         <v>6</v>
       </c>
-      <c r="D45">
-        <v>7</v>
-      </c>
       <c r="E45">
-        <v>9.981373880477658</v>
+        <v>11.33727407175867</v>
       </c>
       <c r="F45">
-        <v>321.8335</v>
+        <v>27.9296</v>
       </c>
       <c r="G45">
-        <v>5.774034331066716</v>
+        <v>3.329687058336451</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1432,22 +1432,22 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46">
-        <v>13.29901660628291</v>
+        <v>5.658956414298633</v>
       </c>
       <c r="F46">
-        <v>199.8239</v>
+        <v>56.19200000000001</v>
       </c>
       <c r="G46">
-        <v>5.297436478680217</v>
+        <v>4.028774398012652</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1455,22 +1455,22 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E47">
-        <v>30.59684981428806</v>
+        <v>5.355006734611161</v>
       </c>
       <c r="F47">
-        <v>135.3036</v>
+        <v>115.489</v>
       </c>
       <c r="G47">
-        <v>4.907521142361571</v>
+        <v>4.749175287331175</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1478,22 +1478,22 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E48">
-        <v>13.74303526717865</v>
+        <v>4.744442981799851</v>
       </c>
       <c r="F48">
-        <v>306.7476</v>
+        <v>17.2925</v>
       </c>
       <c r="G48">
-        <v>5.726025259599533</v>
+        <v>2.850272881492603</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1501,22 +1501,22 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E49">
-        <v>19.86623597126174</v>
+        <v>7.277304068624027</v>
       </c>
       <c r="F49">
-        <v>320.7718</v>
+        <v>14.6372</v>
       </c>
       <c r="G49">
-        <v>5.77072996689156</v>
+        <v>2.683566233410644</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1524,22 +1524,22 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>15.63783182637511</v>
+        <v>14.07929123932978</v>
       </c>
       <c r="F50">
-        <v>251.2358</v>
+        <v>11.269</v>
       </c>
       <c r="G50">
-        <v>5.526391940363181</v>
+        <v>2.422055592970212</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1547,22 +1547,22 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E51">
-        <v>9.976141486413455</v>
+        <v>6.536269697234959</v>
       </c>
       <c r="F51">
-        <v>100.7507</v>
+        <v>82.92650000000003</v>
       </c>
       <c r="G51">
-        <v>4.612649148693475</v>
+        <v>4.417954673303827</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1570,22 +1570,22 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E52">
-        <v>22.94173236544554</v>
+        <v>5.051255061113135</v>
       </c>
       <c r="F52">
-        <v>85.71490000000003</v>
+        <v>159.6970999999999</v>
       </c>
       <c r="G52">
-        <v>4.451026672801819</v>
+        <v>5.073278896007873</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1593,22 +1593,22 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>16.77813957050915</v>
+        <v>4.870323963119561</v>
       </c>
       <c r="F53">
-        <v>89.66429999999998</v>
+        <v>15.5999</v>
       </c>
       <c r="G53">
-        <v>4.496072696533355</v>
+        <v>2.747264503978535</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1616,22 +1616,22 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E54">
-        <v>16.35591123387744</v>
+        <v>6.72385106450545</v>
       </c>
       <c r="F54">
-        <v>64.78819999999999</v>
+        <v>18.10560000000001</v>
       </c>
       <c r="G54">
-        <v>4.171123488010804</v>
+        <v>2.896221282685057</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1639,22 +1639,22 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E55">
-        <v>29.23074389278353</v>
+        <v>8.20149137866404</v>
       </c>
       <c r="F55">
-        <v>65.65070000000001</v>
+        <v>53.4702</v>
       </c>
       <c r="G55">
-        <v>4.184348263296682</v>
+        <v>3.979124489368831</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1662,22 +1662,22 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C56">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E56">
-        <v>21.91645910204142</v>
+        <v>2.965996351305788</v>
       </c>
       <c r="F56">
-        <v>55.36120000000001</v>
+        <v>191.8604</v>
       </c>
       <c r="G56">
-        <v>4.013878987375064</v>
+        <v>5.256768024241167</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1685,22 +1685,22 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C57">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>14.38497122982865</v>
+        <v>5.462159731913236</v>
       </c>
       <c r="F57">
-        <v>82.0806</v>
+        <v>117.7436</v>
       </c>
       <c r="G57">
-        <v>4.407701691337262</v>
+        <v>4.768509378977766</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1708,22 +1708,22 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D58">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>21.02310386990468</v>
+        <v>9.807141259330017</v>
       </c>
       <c r="F58">
-        <v>152.3774</v>
+        <v>110.078</v>
       </c>
       <c r="G58">
-        <v>5.026360338292655</v>
+        <v>4.701189205415331</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1731,22 +1731,22 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C59">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D59">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E59">
-        <v>20.76845057127787</v>
+        <v>5.205813624651588</v>
       </c>
       <c r="F59">
-        <v>162.767</v>
+        <v>200.8036</v>
       </c>
       <c r="G59">
-        <v>5.092319730318768</v>
+        <v>5.302327315943717</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1754,22 +1754,22 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C60">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D60">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E60">
-        <v>16.15161598993626</v>
+        <v>5.957454014211175</v>
       </c>
       <c r="F60">
-        <v>81.23269999999999</v>
+        <v>250.0266</v>
       </c>
       <c r="G60">
-        <v>4.397317875461587</v>
+        <v>5.521567312202168</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1777,22 +1777,22 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C61">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>27.36033772680346</v>
+        <v>4.129199940350803</v>
       </c>
       <c r="F61">
-        <v>86.70910000000003</v>
+        <v>46.7325</v>
       </c>
       <c r="G61">
-        <v>4.462558837909531</v>
+        <v>3.84443985410435</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1800,22 +1800,22 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C62">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E62">
-        <v>21.18800076580996</v>
+        <v>5.320384665371931</v>
       </c>
       <c r="F62">
-        <v>358.9251</v>
+        <v>174.168</v>
       </c>
       <c r="G62">
-        <v>5.883113731623456</v>
+        <v>5.160020350643945</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1823,22 +1823,22 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E63">
-        <v>17.64569507928428</v>
+        <v>3.491384598927763</v>
       </c>
       <c r="F63">
-        <v>153.4061</v>
+        <v>55.1632</v>
       </c>
       <c r="G63">
-        <v>5.033088653461963</v>
+        <v>4.010296064295346</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1846,22 +1846,22 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C64">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E64">
-        <v>22.80083549886487</v>
+        <v>7.470438293247392</v>
       </c>
       <c r="F64">
-        <v>68.29109999999999</v>
+        <v>75.35880000000004</v>
       </c>
       <c r="G64">
-        <v>4.223779450618932</v>
+        <v>4.322260706574448</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1869,22 +1869,22 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C65">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D65">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E65">
-        <v>18.60830368639665</v>
+        <v>6.005983580228081</v>
       </c>
       <c r="F65">
-        <v>188.2735</v>
+        <v>60.4577</v>
       </c>
       <c r="G65">
-        <v>5.237895692886232</v>
+        <v>4.101943946947259</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1892,22 +1892,22 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C66">
+        <v>7</v>
+      </c>
+      <c r="D66">
         <v>10</v>
       </c>
-      <c r="D66">
-        <v>7</v>
-      </c>
       <c r="E66">
-        <v>14.67742729567308</v>
+        <v>5.545553049698621</v>
       </c>
       <c r="F66">
-        <v>389.0132</v>
+        <v>20.9099</v>
       </c>
       <c r="G66">
-        <v>5.963613276204684</v>
+        <v>3.040222731028341</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1915,22 +1915,22 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C67">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D67">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>18.35550041472227</v>
+        <v>6.046118125900827</v>
       </c>
       <c r="F67">
-        <v>159.7623</v>
+        <v>46.98129999999996</v>
       </c>
       <c r="G67">
-        <v>5.073687085598822</v>
+        <v>3.849749650197432</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1938,22 +1938,22 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C68">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E68">
-        <v>24.93203444297038</v>
+        <v>3.761726037138215</v>
       </c>
       <c r="F68">
-        <v>156.8098</v>
+        <v>133.5261</v>
       </c>
       <c r="G68">
-        <v>5.055033605963263</v>
+        <v>4.894296964349548</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1961,22 +1961,22 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C69">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69">
-        <v>23.71562194520213</v>
+        <v>6.683991702498807</v>
       </c>
       <c r="F69">
-        <v>65.20320000000001</v>
+        <v>122.0095</v>
       </c>
       <c r="G69">
-        <v>4.177508547482837</v>
+        <v>4.804098910554094</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1984,22 +1984,22 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C70">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>5.467157935116426</v>
+        <v>3.417035060856205</v>
       </c>
       <c r="F70">
-        <v>226.5258</v>
+        <v>90.47809999999996</v>
       </c>
       <c r="G70">
-        <v>5.422858845720914</v>
+        <v>4.505107832471554</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2007,22 +2007,22 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C71">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E71">
-        <v>32.35271020119843</v>
+        <v>8.421496967200465</v>
       </c>
       <c r="F71">
-        <v>91.092</v>
+        <v>27.2323</v>
       </c>
       <c r="G71">
-        <v>4.511869984822631</v>
+        <v>3.304403768781517</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2030,22 +2030,22 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C72">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D72">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E72">
-        <v>15.19370653578765</v>
+        <v>6.893371161714028</v>
       </c>
       <c r="F72">
-        <v>134.6875</v>
+        <v>15.4005</v>
       </c>
       <c r="G72">
-        <v>4.902957280298067</v>
+        <v>2.734399976424992</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2053,22 +2053,22 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C73">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D73">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E73">
-        <v>21.44964432393407</v>
+        <v>8.166193052756546</v>
       </c>
       <c r="F73">
-        <v>122.8874</v>
+        <v>28.22850000000001</v>
       </c>
       <c r="G73">
-        <v>4.811268488940295</v>
+        <v>3.340332105890881</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2076,22 +2076,22 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C74">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D74">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E74">
-        <v>16.21625112324077</v>
+        <v>2.672106952627844</v>
       </c>
       <c r="F74">
-        <v>72.00720000000001</v>
+        <v>35.0161</v>
       </c>
       <c r="G74">
-        <v>4.276766114016389</v>
+        <v>3.555807955721848</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2099,22 +2099,22 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C75">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D75">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E75">
-        <v>20.84220967181616</v>
+        <v>8.234281370504281</v>
       </c>
       <c r="F75">
-        <v>382.4699</v>
+        <v>8.4468</v>
       </c>
       <c r="G75">
-        <v>5.946649957359691</v>
+        <v>2.133787671419949</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2122,22 +2122,22 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C76">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E76">
-        <v>25.4967962975218</v>
+        <v>9.14356779380174</v>
       </c>
       <c r="F76">
-        <v>43.2142</v>
+        <v>33.80399999999997</v>
       </c>
       <c r="G76">
-        <v>3.766169144942541</v>
+        <v>3.520579138682235</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2145,22 +2145,22 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C77">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D77">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E77">
-        <v>16.03891012677666</v>
+        <v>7.525087877315707</v>
       </c>
       <c r="F77">
-        <v>61.31960000000001</v>
+        <v>66.68150000000007</v>
       </c>
       <c r="G77">
-        <v>4.11609953082513</v>
+        <v>4.199927553130475</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2168,22 +2168,22 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C78">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E78">
-        <v>17.42133360814174</v>
+        <v>7.713880325743857</v>
       </c>
       <c r="F78">
-        <v>99.07459999999999</v>
+        <v>52.80629999999999</v>
       </c>
       <c r="G78">
-        <v>4.595873101722903</v>
+        <v>3.966630501776186</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2191,22 +2191,22 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C79">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D79">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E79">
-        <v>13.56203763400632</v>
+        <v>7.581946573007931</v>
       </c>
       <c r="F79">
-        <v>115.0226</v>
+        <v>80.50449999999999</v>
       </c>
       <c r="G79">
-        <v>4.745128630794513</v>
+        <v>4.388313083483254</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2214,22 +2214,22 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C80">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E80">
-        <v>27.04348880002225</v>
+        <v>5.576870486326129</v>
       </c>
       <c r="F80">
-        <v>158.7182</v>
+        <v>13.4757</v>
       </c>
       <c r="G80">
-        <v>5.06713030274645</v>
+        <v>2.600888063497755</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2237,22 +2237,22 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C81">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E81">
-        <v>15.57825617977681</v>
+        <v>11.01526578681647</v>
       </c>
       <c r="F81">
-        <v>216.005</v>
+        <v>85.98210000000002</v>
       </c>
       <c r="G81">
-        <v>5.375301555564399</v>
+        <v>4.454139135054585</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2260,22 +2260,22 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C82">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E82">
-        <v>14.31629498716925</v>
+        <v>8.692715109657463</v>
       </c>
       <c r="F82">
-        <v>189.5521</v>
+        <v>119.4853</v>
       </c>
       <c r="G82">
-        <v>5.244663920771984</v>
+        <v>4.783193351252599</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2283,22 +2283,22 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C83">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D83">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E83">
-        <v>14.90082732228793</v>
+        <v>8.544807491409404</v>
       </c>
       <c r="F83">
-        <v>89.21610000000001</v>
+        <v>57.3188</v>
       </c>
       <c r="G83">
-        <v>4.491061516572556</v>
+        <v>4.048628667639642</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2306,22 +2306,22 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C84">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D84">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E84">
-        <v>14.40371889215392</v>
+        <v>9.204960114625187</v>
       </c>
       <c r="F84">
-        <v>412.2123</v>
+        <v>11.9994</v>
       </c>
       <c r="G84">
-        <v>6.02153850789471</v>
+        <v>2.484856648537959</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2329,22 +2329,22 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C85">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D85">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>10.10057333208464</v>
+        <v>7.736680665124612</v>
       </c>
       <c r="F85">
-        <v>167.3145</v>
+        <v>109.312</v>
       </c>
       <c r="G85">
-        <v>5.119875274888619</v>
+        <v>4.69420617872605</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2352,22 +2352,22 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C86">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86">
-        <v>9.334242035685341</v>
+        <v>9.348324768308343</v>
       </c>
       <c r="F86">
-        <v>118.1591</v>
+        <v>204.5204999999999</v>
       </c>
       <c r="G86">
-        <v>4.772032021403324</v>
+        <v>5.32066821495749</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2375,22 +2375,22 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C87">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E87">
-        <v>5.446534220587725</v>
+        <v>6.491867540585763</v>
       </c>
       <c r="F87">
-        <v>70.099</v>
+        <v>118.1418</v>
       </c>
       <c r="G87">
-        <v>4.249908528603558</v>
+        <v>4.771885597923507</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2398,22 +2398,22 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C88">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D88">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E88">
-        <v>18.61070510227305</v>
+        <v>11.69696886298522</v>
       </c>
       <c r="F88">
-        <v>63.56019999999999</v>
+        <v>53.7871</v>
       </c>
       <c r="G88">
-        <v>4.151987488296667</v>
+        <v>3.985033661464977</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2421,22 +2421,22 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C89">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D89">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E89">
-        <v>2.225766708967556</v>
+        <v>6.573445341075474</v>
       </c>
       <c r="F89">
-        <v>121.8924</v>
+        <v>147.3818</v>
       </c>
       <c r="G89">
-        <v>4.803138688358223</v>
+        <v>4.993026498590367</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2444,22 +2444,22 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C90">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D90">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E90">
-        <v>7.487689304349217</v>
+        <v>8.259263936558479</v>
       </c>
       <c r="F90">
-        <v>160.9415</v>
+        <v>37.5551</v>
       </c>
       <c r="G90">
-        <v>5.081040944918122</v>
+        <v>3.625809187895713</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2467,22 +2467,22 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C91">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D91">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E91">
-        <v>11.72498313374156</v>
+        <v>5.454610312406809</v>
       </c>
       <c r="F91">
-        <v>53.4038</v>
+        <v>192.3592</v>
       </c>
       <c r="G91">
-        <v>3.977881904483011</v>
+        <v>5.259364457532026</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2490,22 +2490,22 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C92">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E92">
-        <v>12.32024647784447</v>
+        <v>7.076247200942581</v>
       </c>
       <c r="F92">
-        <v>79.60820000000001</v>
+        <v>81.2825</v>
       </c>
       <c r="G92">
-        <v>4.377117102620026</v>
+        <v>4.397930741231174</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2513,22 +2513,22 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C93">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E93">
-        <v>13.03011789105975</v>
+        <v>10.04224931399291</v>
       </c>
       <c r="F93">
-        <v>281.9879</v>
+        <v>61.58569999999999</v>
       </c>
       <c r="G93">
-        <v>5.641864162216129</v>
+        <v>4.120429700733007</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2536,22 +2536,22 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C94">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D94">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E94">
-        <v>13.10790329081541</v>
+        <v>6.703763437805576</v>
       </c>
       <c r="F94">
-        <v>137.0946</v>
+        <v>45.1567</v>
       </c>
       <c r="G94">
-        <v>4.920671198484034</v>
+        <v>3.810138663095076</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2559,22 +2559,22 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C95">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D95">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E95">
-        <v>12.88186787685873</v>
+        <v>4.762672242224308</v>
       </c>
       <c r="F95">
-        <v>149.4577</v>
+        <v>143.5005000000001</v>
       </c>
       <c r="G95">
-        <v>5.007013409650965</v>
+        <v>4.966338519514164</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2582,22 +2582,22 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C96">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D96">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E96">
-        <v>9.147100609773819</v>
+        <v>3.095987526983857</v>
       </c>
       <c r="F96">
-        <v>153.5565</v>
+        <v>167.9443</v>
       </c>
       <c r="G96">
-        <v>5.034068577478994</v>
+        <v>5.123632376810148</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2605,22 +2605,22 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C97">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E97">
-        <v>22.05898719880597</v>
+        <v>8.073901628955353</v>
       </c>
       <c r="F97">
-        <v>78.71169999999998</v>
+        <v>204.0233</v>
       </c>
       <c r="G97">
-        <v>4.365791810193257</v>
+        <v>5.318234203008376</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2628,22 +2628,22 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C98">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E98">
-        <v>8.178189795239998</v>
+        <v>6.064865155994274</v>
       </c>
       <c r="F98">
-        <v>117.578</v>
+        <v>94.67599999999997</v>
       </c>
       <c r="G98">
-        <v>4.767101943133916</v>
+        <v>4.550460536182564</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2651,22 +2651,22 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C99">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E99">
-        <v>11.53613566998474</v>
+        <v>6.635981299232818</v>
       </c>
       <c r="F99">
-        <v>352.2523</v>
+        <v>173.6864</v>
       </c>
       <c r="G99">
-        <v>5.864347680210986</v>
+        <v>5.157251374269282</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2674,22 +2674,22 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C100">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D100">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E100">
-        <v>9.094091628423238</v>
+        <v>6.372077026605698</v>
       </c>
       <c r="F100">
-        <v>93.8301</v>
+        <v>52.0758</v>
       </c>
       <c r="G100">
-        <v>4.541485700058611</v>
+        <v>3.952700349487027</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2697,22 +2697,22 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C101">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D101">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E101">
-        <v>8.699198868236063</v>
+        <v>6.901031772418647</v>
       </c>
       <c r="F101">
-        <v>85.0343</v>
+        <v>305.5509999999999</v>
       </c>
       <c r="G101">
-        <v>4.443054704505984</v>
+        <v>5.722116704122347</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2720,22 +2720,22 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C102">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E102">
-        <v>8.48420789654233</v>
+        <v>8.466495126934248</v>
       </c>
       <c r="F102">
-        <v>100.7335</v>
+        <v>174.7332</v>
       </c>
       <c r="G102">
-        <v>4.612478415702582</v>
+        <v>5.163260239153374</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2743,22 +2743,22 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C103">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D103">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E103">
-        <v>11.46752678278714</v>
+        <v>8.919466319630333</v>
       </c>
       <c r="F103">
-        <v>147.3001</v>
+        <v>93.8135</v>
       </c>
       <c r="G103">
-        <v>4.99247200235498</v>
+        <v>4.541308768897161</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2766,22 +2766,22 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C104">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D104">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E104">
-        <v>11.74852963457179</v>
+        <v>7.016502468297869</v>
       </c>
       <c r="F104">
-        <v>121.1956</v>
+        <v>76.60429999999999</v>
       </c>
       <c r="G104">
-        <v>4.797405769345858</v>
+        <v>4.338653210941227</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2789,22 +2789,22 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C105">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E105">
-        <v>15.01741120743734</v>
+        <v>4.193501768762057</v>
       </c>
       <c r="F105">
-        <v>239.6704</v>
+        <v>11.7995</v>
       </c>
       <c r="G105">
-        <v>5.479264646122156</v>
+        <v>2.468057157692507</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2812,22 +2812,22 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C106">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D106">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E106">
-        <v>15.30004742129951</v>
+        <v>18.11683952192893</v>
       </c>
       <c r="F106">
-        <v>92.7355</v>
+        <v>16.9765</v>
       </c>
       <c r="G106">
-        <v>4.529751355034269</v>
+        <v>2.831830034783786</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2835,22 +2835,22 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C107">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D107">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E107">
-        <v>21.15792468376722</v>
+        <v>16.39459342873933</v>
       </c>
       <c r="F107">
-        <v>148.6614</v>
+        <v>12.7122</v>
       </c>
       <c r="G107">
-        <v>5.001671236715469</v>
+        <v>2.542562162276163</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2858,22 +2858,22 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C108">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D108">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E108">
-        <v>12.71097281332166</v>
+        <v>13.14228853056053</v>
       </c>
       <c r="F108">
-        <v>181.8022</v>
+        <v>7.5676</v>
       </c>
       <c r="G108">
-        <v>5.202919282880281</v>
+        <v>2.023875976230127</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2881,22 +2881,22 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C109">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D109">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E109">
-        <v>22.26673786279014</v>
+        <v>4.732935537513954</v>
       </c>
       <c r="F109">
-        <v>162.884</v>
+        <v>39.116</v>
       </c>
       <c r="G109">
-        <v>5.093038291017394</v>
+        <v>3.666531590450029</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2904,22 +2904,22 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C110">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D110">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E110">
-        <v>24.68423745458491</v>
+        <v>7.477521131435365</v>
       </c>
       <c r="F110">
-        <v>97.49670000000002</v>
+        <v>17.02709999999998</v>
       </c>
       <c r="G110">
-        <v>4.579818531277161</v>
+        <v>2.834806192446455</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2927,22 +2927,22 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C111">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E111">
-        <v>7.980311441483169</v>
+        <v>12.8423037422803</v>
       </c>
       <c r="F111">
-        <v>94.42700000000001</v>
+        <v>12.2145</v>
       </c>
       <c r="G111">
-        <v>4.547827049205558</v>
+        <v>2.502623770593158</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2950,22 +2950,22 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C112">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>9.461886175295573</v>
+        <v>7.738348253218916</v>
       </c>
       <c r="F112">
-        <v>84.0215</v>
+        <v>163.2476</v>
       </c>
       <c r="G112">
-        <v>4.431072718474043</v>
+        <v>5.095268066670219</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2973,22 +2973,22 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C113">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E113">
-        <v>7.573283695994116</v>
+        <v>6.036686669667413</v>
       </c>
       <c r="F113">
-        <v>359.721</v>
+        <v>271.4158</v>
       </c>
       <c r="G113">
-        <v>5.885328730982404</v>
+        <v>5.60365196236063</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -2996,22 +2996,22 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C114">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D114">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E114">
-        <v>9.226095863083136</v>
+        <v>5.550774527260953</v>
       </c>
       <c r="F114">
-        <v>74.77809999999999</v>
+        <v>176.508</v>
       </c>
       <c r="G114">
-        <v>4.314525061363117</v>
+        <v>5.173366201125206</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3019,22 +3019,22 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C115">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D115">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E115">
-        <v>10.84239503979799</v>
+        <v>2.576547053696279</v>
       </c>
       <c r="F115">
-        <v>258.1728</v>
+        <v>32.8913</v>
       </c>
       <c r="G115">
-        <v>5.553629128169365</v>
+        <v>3.493208185111546</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3042,22 +3042,22 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C116">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D116">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E116">
-        <v>2.355408302586286</v>
+        <v>4.604533581078821</v>
       </c>
       <c r="F116">
-        <v>125.8093</v>
+        <v>77.7159</v>
       </c>
       <c r="G116">
-        <v>4.834767268401928</v>
+        <v>4.353059869643717</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3065,22 +3065,22 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C117">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E117">
-        <v>25.54723215202756</v>
+        <v>4.410725730935523</v>
       </c>
       <c r="F117">
-        <v>114.5573</v>
+        <v>64.60540000000002</v>
       </c>
       <c r="G117">
-        <v>4.741075134498842</v>
+        <v>4.168297998626265</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3088,22 +3088,22 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C118">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D118">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E118">
-        <v>21.94893368557131</v>
+        <v>5.008806197865224</v>
       </c>
       <c r="F118">
-        <v>71.6254</v>
+        <v>285.7886</v>
       </c>
       <c r="G118">
-        <v>4.271449759661543</v>
+        <v>5.655252376666628</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3111,22 +3111,22 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C119">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D119">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E119">
-        <v>11.07334955566618</v>
+        <v>5.441134370872109</v>
       </c>
       <c r="F119">
-        <v>102.1111</v>
+        <v>109.2644999999999</v>
       </c>
       <c r="G119">
-        <v>4.626061436205534</v>
+        <v>4.693771548280894</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3134,22 +3134,22 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C120">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D120">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E120">
-        <v>11.88841732521326</v>
+        <v>7.272902672014418</v>
       </c>
       <c r="F120">
-        <v>115.3375</v>
+        <v>64.07469999999999</v>
       </c>
       <c r="G120">
-        <v>4.747862612904674</v>
+        <v>4.160049590225908</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3157,22 +3157,22 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C121">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D121">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E121">
-        <v>14.31515008406149</v>
+        <v>1.070625072668587</v>
       </c>
       <c r="F121">
-        <v>86.04630000000002</v>
+        <v>26.1374</v>
       </c>
       <c r="G121">
-        <v>4.454885523476269</v>
+        <v>3.263367238826821</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3180,22 +3180,22 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C122">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D122">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>19.59524630275981</v>
+        <v>4.507268622759054</v>
       </c>
       <c r="F122">
-        <v>116.9633</v>
+        <v>24.71050000000001</v>
       </c>
       <c r="G122">
-        <v>4.761860210377721</v>
+        <v>3.207228254518584</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3203,22 +3203,22 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C123">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D123">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E123">
-        <v>12.59484169372528</v>
+        <v>3.076292450046231</v>
       </c>
       <c r="F123">
-        <v>170.9653</v>
+        <v>81.35079999999995</v>
       </c>
       <c r="G123">
-        <v>5.141460611934196</v>
+        <v>4.398770667667092</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3226,22 +3226,22 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C124">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D124">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E124">
-        <v>7.936724596848236</v>
+        <v>3.980575511052577</v>
       </c>
       <c r="F124">
-        <v>221.763</v>
+        <v>188.5571</v>
       </c>
       <c r="G124">
-        <v>5.401609244048562</v>
+        <v>5.239400878789623</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3249,22 +3249,22 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C125">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D125">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E125">
-        <v>21.58922562026961</v>
+        <v>9.297932836765471</v>
       </c>
       <c r="F125">
-        <v>108.417</v>
+        <v>39.7784</v>
       </c>
       <c r="G125">
-        <v>4.685984903277811</v>
+        <v>3.683324051400239</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3272,22 +3272,22 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C126">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D126">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E126">
-        <v>9.779072714623322</v>
+        <v>3.051328323981361</v>
       </c>
       <c r="F126">
-        <v>127.9831</v>
+        <v>106.2931</v>
       </c>
       <c r="G126">
-        <v>4.851898223952724</v>
+        <v>4.666200372610825</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3295,22 +3295,22 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C127">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D127">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E127">
-        <v>8.995342027850779</v>
+        <v>4.758227239145203</v>
       </c>
       <c r="F127">
-        <v>82.3133</v>
+        <v>48.77290000000001</v>
       </c>
       <c r="G127">
-        <v>4.410532698514737</v>
+        <v>3.887174830738619</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3318,22 +3318,22 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C128">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D128">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E128">
-        <v>8.359266750930475</v>
+        <v>4.095262946088554</v>
       </c>
       <c r="F128">
-        <v>123.6353</v>
+        <v>126.9045</v>
       </c>
       <c r="G128">
-        <v>4.817336102953545</v>
+        <v>4.843434835084524</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3341,22 +3341,1425 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="C129">
+        <v>14</v>
+      </c>
+      <c r="D129">
+        <v>8</v>
+      </c>
+      <c r="E129">
+        <v>4.132817927311165</v>
+      </c>
+      <c r="F129">
+        <v>55.04660000000002</v>
+      </c>
+      <c r="G129">
+        <v>4.008180099226823</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>3000</v>
+      </c>
+      <c r="C130">
+        <v>14</v>
+      </c>
+      <c r="D130">
+        <v>9</v>
+      </c>
+      <c r="E130">
+        <v>3.687734294592177</v>
+      </c>
+      <c r="F130">
+        <v>91.02550000000001</v>
+      </c>
+      <c r="G130">
+        <v>4.51113968704284</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>3000</v>
+      </c>
+      <c r="C131">
+        <v>14</v>
+      </c>
+      <c r="D131">
+        <v>10</v>
+      </c>
+      <c r="E131">
+        <v>3.605052019198201</v>
+      </c>
+      <c r="F131">
+        <v>47.89400000000001</v>
+      </c>
+      <c r="G131">
+        <v>3.868990235610726</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>3000</v>
+      </c>
+      <c r="C132">
+        <v>15</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>14.67271197973974</v>
+      </c>
+      <c r="F132">
+        <v>18.5702</v>
+      </c>
+      <c r="G132">
+        <v>2.921558145365853</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>3000</v>
+      </c>
+      <c r="C133">
+        <v>15</v>
+      </c>
+      <c r="D133">
+        <v>2</v>
+      </c>
+      <c r="E133">
+        <v>3.379065042822609</v>
+      </c>
+      <c r="F133">
+        <v>72.02419999999999</v>
+      </c>
+      <c r="G133">
+        <v>4.277002173654481</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>3000</v>
+      </c>
+      <c r="C134">
+        <v>15</v>
+      </c>
+      <c r="D134">
+        <v>3</v>
+      </c>
+      <c r="E134">
+        <v>5.261129175406723</v>
+      </c>
+      <c r="F134">
+        <v>160.9755</v>
+      </c>
+      <c r="G134">
+        <v>5.081252179491795</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>3000</v>
+      </c>
+      <c r="C135">
+        <v>15</v>
+      </c>
+      <c r="D135">
+        <v>4</v>
+      </c>
+      <c r="E135">
+        <v>3.656704640419241</v>
+      </c>
+      <c r="F135">
+        <v>87.34139999999999</v>
+      </c>
+      <c r="G135">
+        <v>4.469824577239686</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>3000</v>
+      </c>
+      <c r="C136">
+        <v>15</v>
+      </c>
+      <c r="D136">
+        <v>5</v>
+      </c>
+      <c r="E136">
+        <v>4.108217558954789</v>
+      </c>
+      <c r="F136">
+        <v>50.78120000000001</v>
+      </c>
+      <c r="G136">
+        <v>3.927526207348242</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>3000</v>
+      </c>
+      <c r="C137">
+        <v>15</v>
+      </c>
+      <c r="D137">
+        <v>6</v>
+      </c>
+      <c r="E137">
+        <v>8.06876671646757</v>
+      </c>
+      <c r="F137">
+        <v>13.6581</v>
+      </c>
+      <c r="G137">
+        <v>2.614332752228304</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>3000</v>
+      </c>
+      <c r="C138">
+        <v>15</v>
+      </c>
+      <c r="D138">
+        <v>7</v>
+      </c>
+      <c r="E138">
+        <v>4.310971011679326</v>
+      </c>
+      <c r="F138">
+        <v>72.63719999999999</v>
+      </c>
+      <c r="G138">
+        <v>4.285477187294605</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>3000</v>
+      </c>
+      <c r="C139">
+        <v>15</v>
+      </c>
+      <c r="D139">
+        <v>8</v>
+      </c>
+      <c r="E139">
+        <v>3.573826230785755</v>
+      </c>
+      <c r="F139">
+        <v>67.09509999999997</v>
+      </c>
+      <c r="G139">
+        <v>4.206111015975836</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>3000</v>
+      </c>
+      <c r="C140">
+        <v>15</v>
+      </c>
+      <c r="D140">
+        <v>9</v>
+      </c>
+      <c r="E140">
+        <v>6.585691000504453</v>
+      </c>
+      <c r="F140">
+        <v>11.0194</v>
+      </c>
+      <c r="G140">
+        <v>2.399657355781526</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>3000</v>
+      </c>
+      <c r="C141">
+        <v>16</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>7.761087588846698</v>
+      </c>
+      <c r="F141">
+        <v>83.87229999999997</v>
+      </c>
+      <c r="G141">
+        <v>4.429295404013653</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>3000</v>
+      </c>
+      <c r="C142">
+        <v>16</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+      <c r="E142">
+        <v>3.389123977244255</v>
+      </c>
+      <c r="F142">
+        <v>106.4755</v>
+      </c>
+      <c r="G142">
+        <v>4.667914911736265</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>3000</v>
+      </c>
+      <c r="C143">
+        <v>16</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
+        <v>4.649723101889768</v>
+      </c>
+      <c r="F143">
+        <v>205.1345999999999</v>
+      </c>
+      <c r="G143">
+        <v>5.323666349046396</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>3000</v>
+      </c>
+      <c r="C144">
+        <v>16</v>
+      </c>
+      <c r="D144">
+        <v>4</v>
+      </c>
+      <c r="E144">
+        <v>7.779413403946918</v>
+      </c>
+      <c r="F144">
+        <v>6.8716</v>
+      </c>
+      <c r="G144">
+        <v>1.927396975770153</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>3000</v>
+      </c>
+      <c r="C145">
+        <v>16</v>
+      </c>
+      <c r="D145">
+        <v>5</v>
+      </c>
+      <c r="E145">
+        <v>7.247208649111275</v>
+      </c>
+      <c r="F145">
+        <v>34.83370000000003</v>
+      </c>
+      <c r="G145">
+        <v>3.550585308997145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>3000</v>
+      </c>
+      <c r="C146">
+        <v>16</v>
+      </c>
+      <c r="D146">
+        <v>6</v>
+      </c>
+      <c r="E146">
+        <v>6.716571338535719</v>
+      </c>
+      <c r="F146">
+        <v>11.8659</v>
+      </c>
+      <c r="G146">
+        <v>2.473668740361197</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>3000</v>
+      </c>
+      <c r="C147">
+        <v>16</v>
+      </c>
+      <c r="D147">
+        <v>7</v>
+      </c>
+      <c r="E147">
+        <v>4.394616811139308</v>
+      </c>
+      <c r="F147">
+        <v>52.60780000000002</v>
+      </c>
+      <c r="G147">
+        <v>3.962864397723326</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>3000</v>
+      </c>
+      <c r="C148">
+        <v>16</v>
+      </c>
+      <c r="D148">
+        <v>8</v>
+      </c>
+      <c r="E148">
+        <v>5.745003735089632</v>
+      </c>
+      <c r="F148">
+        <v>48.85620000000001</v>
+      </c>
+      <c r="G148">
+        <v>3.888881289575465</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>3000</v>
+      </c>
+      <c r="C149">
+        <v>16</v>
+      </c>
+      <c r="D149">
+        <v>9</v>
+      </c>
+      <c r="E149">
+        <v>2.532631639017824</v>
+      </c>
+      <c r="F149">
+        <v>13.376</v>
+      </c>
+      <c r="G149">
+        <v>2.593462056342346</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>3000</v>
+      </c>
+      <c r="C150">
+        <v>16</v>
+      </c>
+      <c r="D150">
+        <v>10</v>
+      </c>
+      <c r="E150">
+        <v>5.908509370739187</v>
+      </c>
+      <c r="F150">
+        <v>8.115</v>
+      </c>
+      <c r="G150">
+        <v>2.093714200966554</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>3000</v>
+      </c>
+      <c r="C151">
+        <v>17</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>6.765581262913956</v>
+      </c>
+      <c r="F151">
+        <v>29.0578</v>
+      </c>
+      <c r="G151">
+        <v>3.369286949839309</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>3000</v>
+      </c>
+      <c r="C152">
+        <v>17</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152">
+        <v>4.388551395238449</v>
+      </c>
+      <c r="F152">
+        <v>67.64180000000002</v>
+      </c>
+      <c r="G152">
+        <v>4.214226135148802</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>3000</v>
+      </c>
+      <c r="C153">
+        <v>17</v>
+      </c>
+      <c r="D153">
+        <v>3</v>
+      </c>
+      <c r="E153">
+        <v>3.773565374663945</v>
+      </c>
+      <c r="F153">
+        <v>89.73070000000001</v>
+      </c>
+      <c r="G153">
+        <v>4.496812962460859</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>3000</v>
+      </c>
+      <c r="C154">
+        <v>17</v>
+      </c>
+      <c r="D154">
+        <v>4</v>
+      </c>
+      <c r="E154">
+        <v>4.011887909146466</v>
+      </c>
+      <c r="F154">
+        <v>95.15730000000001</v>
+      </c>
+      <c r="G154">
+        <v>4.55553131176615</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>3000</v>
+      </c>
+      <c r="C155">
+        <v>17</v>
+      </c>
+      <c r="D155">
+        <v>5</v>
+      </c>
+      <c r="E155">
+        <v>6.120200024434715</v>
+      </c>
+      <c r="F155">
+        <v>137.5245</v>
+      </c>
+      <c r="G155">
+        <v>4.923802083052313</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>3000</v>
+      </c>
+      <c r="C156">
+        <v>17</v>
+      </c>
+      <c r="D156">
+        <v>6</v>
+      </c>
+      <c r="E156">
+        <v>4.600176697105304</v>
+      </c>
+      <c r="F156">
+        <v>45.1233</v>
+      </c>
+      <c r="G156">
+        <v>3.809398742813201</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>3000</v>
+      </c>
+      <c r="C157">
+        <v>17</v>
+      </c>
+      <c r="D157">
+        <v>7</v>
+      </c>
+      <c r="E157">
+        <v>6.608961134033142</v>
+      </c>
+      <c r="F157">
+        <v>95.19139999999999</v>
+      </c>
+      <c r="G157">
+        <v>4.555889601582312</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>3000</v>
+      </c>
+      <c r="C158">
+        <v>17</v>
+      </c>
+      <c r="D158">
+        <v>8</v>
+      </c>
+      <c r="E158">
+        <v>3.952352811876337</v>
+      </c>
+      <c r="F158">
+        <v>108.7668</v>
+      </c>
+      <c r="G158">
+        <v>4.689206140796181</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>3000</v>
+      </c>
+      <c r="C159">
+        <v>17</v>
+      </c>
+      <c r="D159">
+        <v>9</v>
+      </c>
+      <c r="E159">
+        <v>8.712802889380317</v>
+      </c>
+      <c r="F159">
+        <v>70.97929999999999</v>
+      </c>
+      <c r="G159">
+        <v>4.262388285236782</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>3000</v>
+      </c>
+      <c r="C160">
+        <v>17</v>
+      </c>
+      <c r="D160">
+        <v>10</v>
+      </c>
+      <c r="E160">
+        <v>4.959417601433316</v>
+      </c>
+      <c r="F160">
+        <v>66.09859999999998</v>
+      </c>
+      <c r="G160">
+        <v>4.191147566603083</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>3000</v>
+      </c>
+      <c r="C161">
+        <v>18</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>2.35238515934649</v>
+      </c>
+      <c r="F161">
+        <v>74.97829999999999</v>
+      </c>
+      <c r="G161">
+        <v>4.317198738338012</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>3000</v>
+      </c>
+      <c r="C162">
+        <v>18</v>
+      </c>
+      <c r="D162">
+        <v>2</v>
+      </c>
+      <c r="E162">
+        <v>2.853729948973903</v>
+      </c>
+      <c r="F162">
+        <v>140.414</v>
+      </c>
+      <c r="G162">
+        <v>4.944595201720206</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>3000</v>
+      </c>
+      <c r="C163">
+        <v>18</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+      <c r="E163">
+        <v>2.386487545619942</v>
+      </c>
+      <c r="F163">
+        <v>162.9995</v>
+      </c>
+      <c r="G163">
+        <v>5.093747133317395</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>3000</v>
+      </c>
+      <c r="C164">
+        <v>18</v>
+      </c>
+      <c r="D164">
+        <v>4</v>
+      </c>
+      <c r="E164">
+        <v>3.190047276142429</v>
+      </c>
+      <c r="F164">
+        <v>46.93109999999999</v>
+      </c>
+      <c r="G164">
+        <v>3.848680568696346</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>3000</v>
+      </c>
+      <c r="C165">
+        <v>18</v>
+      </c>
+      <c r="D165">
+        <v>5</v>
+      </c>
+      <c r="E165">
+        <v>4.364034199163878</v>
+      </c>
+      <c r="F165">
+        <v>52.3745</v>
+      </c>
+      <c r="G165">
+        <v>3.958419831657354</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>3000</v>
+      </c>
+      <c r="C166">
+        <v>18</v>
+      </c>
+      <c r="D166">
+        <v>6</v>
+      </c>
+      <c r="E166">
+        <v>3.186137071036813</v>
+      </c>
+      <c r="F166">
+        <v>52.49099999999999</v>
+      </c>
+      <c r="G166">
+        <v>3.960641726330592</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>3000</v>
+      </c>
+      <c r="C167">
+        <v>18</v>
+      </c>
+      <c r="D167">
+        <v>7</v>
+      </c>
+      <c r="E167">
+        <v>3.038450871464664</v>
+      </c>
+      <c r="F167">
+        <v>120.6146</v>
+      </c>
+      <c r="G167">
+        <v>4.792600338325617</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>3000</v>
+      </c>
+      <c r="C168">
+        <v>18</v>
+      </c>
+      <c r="D168">
+        <v>8</v>
+      </c>
+      <c r="E168">
+        <v>8.665393300224602</v>
+      </c>
+      <c r="F168">
+        <v>30.08689999999999</v>
+      </c>
+      <c r="G168">
+        <v>3.404089861074038</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>3000</v>
+      </c>
+      <c r="C169">
+        <v>18</v>
+      </c>
+      <c r="D169">
+        <v>9</v>
+      </c>
+      <c r="E169">
+        <v>7.471309987969309</v>
+      </c>
+      <c r="F169">
+        <v>29.72300000000002</v>
+      </c>
+      <c r="G169">
+        <v>3.39192115688176</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>3000</v>
+      </c>
+      <c r="C170">
+        <v>18</v>
+      </c>
+      <c r="D170">
+        <v>10</v>
+      </c>
+      <c r="E170">
+        <v>2.813294513249073</v>
+      </c>
+      <c r="F170">
+        <v>29.2406</v>
+      </c>
+      <c r="G170">
+        <v>3.37555815450689</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>3000</v>
+      </c>
+      <c r="C171">
+        <v>19</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>7.78481877406089</v>
+      </c>
+      <c r="F171">
+        <v>83.9079</v>
+      </c>
+      <c r="G171">
+        <v>4.429719768754358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" s="1">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>3000</v>
+      </c>
+      <c r="C172">
+        <v>19</v>
+      </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
+      <c r="E172">
+        <v>6.089292079015795</v>
+      </c>
+      <c r="F172">
+        <v>113.5951</v>
+      </c>
+      <c r="G172">
+        <v>4.732640371553945</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" s="1">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>3000</v>
+      </c>
+      <c r="C173">
+        <v>19</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>3.575936882860741</v>
+      </c>
+      <c r="F173">
+        <v>187.3123999999999</v>
+      </c>
+      <c r="G173">
+        <v>5.232777811209538</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" s="1">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>3000</v>
+      </c>
+      <c r="C174">
+        <v>19</v>
+      </c>
+      <c r="D174">
+        <v>4</v>
+      </c>
+      <c r="E174">
+        <v>6.223838624639669</v>
+      </c>
+      <c r="F174">
+        <v>53.8186</v>
+      </c>
+      <c r="G174">
+        <v>3.985619132325717</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" s="1">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>3000</v>
+      </c>
+      <c r="C175">
+        <v>19</v>
+      </c>
+      <c r="D175">
+        <v>5</v>
+      </c>
+      <c r="E175">
+        <v>5.419056723366921</v>
+      </c>
+      <c r="F175">
+        <v>138.0055</v>
+      </c>
+      <c r="G175">
+        <v>4.927293539435476</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" s="1">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>3000</v>
+      </c>
+      <c r="C176">
+        <v>19</v>
+      </c>
+      <c r="D176">
+        <v>6</v>
+      </c>
+      <c r="E176">
+        <v>6.818780101599003</v>
+      </c>
+      <c r="F176">
+        <v>74.9114</v>
+      </c>
+      <c r="G176">
+        <v>4.316306081878731</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" s="1">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>3000</v>
+      </c>
+      <c r="C177">
+        <v>19</v>
+      </c>
+      <c r="D177">
+        <v>7</v>
+      </c>
+      <c r="E177">
+        <v>4.483160665894721</v>
+      </c>
+      <c r="F177">
+        <v>117.1634</v>
+      </c>
+      <c r="G177">
+        <v>4.76356954168185</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" s="1">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>3000</v>
+      </c>
+      <c r="C178">
+        <v>19</v>
+      </c>
+      <c r="D178">
+        <v>8</v>
+      </c>
+      <c r="E178">
+        <v>3.517895355555947</v>
+      </c>
+      <c r="F178">
+        <v>109.38</v>
+      </c>
+      <c r="G178">
+        <v>4.694828057918627</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" s="1">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>3000</v>
+      </c>
+      <c r="C179">
+        <v>19</v>
+      </c>
+      <c r="D179">
+        <v>9</v>
+      </c>
+      <c r="E179">
+        <v>14.40597606191969</v>
+      </c>
+      <c r="F179">
+        <v>32.1283</v>
+      </c>
+      <c r="G179">
+        <v>3.469737261675071</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" s="1">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>3000</v>
+      </c>
+      <c r="C180">
+        <v>19</v>
+      </c>
+      <c r="D180">
+        <v>10</v>
+      </c>
+      <c r="E180">
+        <v>3.66417814965925</v>
+      </c>
+      <c r="F180">
+        <v>83.52370000000002</v>
+      </c>
+      <c r="G180">
+        <v>4.425130423919362</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" s="1">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>3000</v>
+      </c>
+      <c r="C181">
         <v>20</v>
       </c>
-      <c r="D129">
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>7.300463750464545</v>
+      </c>
+      <c r="F181">
+        <v>30.71810000000001</v>
+      </c>
+      <c r="G181">
+        <v>3.424852057408413</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" s="1">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>3000</v>
+      </c>
+      <c r="C182">
+        <v>20</v>
+      </c>
+      <c r="D182">
+        <v>2</v>
+      </c>
+      <c r="E182">
+        <v>3.581052331138435</v>
+      </c>
+      <c r="F182">
+        <v>81.84720000000002</v>
+      </c>
+      <c r="G182">
+        <v>4.404854094313252</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" s="1">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>3000</v>
+      </c>
+      <c r="C183">
+        <v>20</v>
+      </c>
+      <c r="D183">
+        <v>3</v>
+      </c>
+      <c r="E183">
+        <v>4.213201422125447</v>
+      </c>
+      <c r="F183">
+        <v>46.2354</v>
+      </c>
+      <c r="G183">
+        <v>3.833745738446704</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" s="1">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>3000</v>
+      </c>
+      <c r="C184">
+        <v>20</v>
+      </c>
+      <c r="D184">
+        <v>4</v>
+      </c>
+      <c r="E184">
+        <v>5.599271804086913</v>
+      </c>
+      <c r="F184">
+        <v>45.33819999999999</v>
+      </c>
+      <c r="G184">
+        <v>3.814149944247204</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" s="1">
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <v>3000</v>
+      </c>
+      <c r="C185">
+        <v>20</v>
+      </c>
+      <c r="D185">
+        <v>5</v>
+      </c>
+      <c r="E185">
+        <v>9.131589475112904</v>
+      </c>
+      <c r="F185">
+        <v>28.46099999999999</v>
+      </c>
+      <c r="G185">
+        <v>3.348534729078849</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" s="1">
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <v>3000</v>
+      </c>
+      <c r="C186">
+        <v>20</v>
+      </c>
+      <c r="D186">
+        <v>6</v>
+      </c>
+      <c r="E186">
+        <v>3.0187463067828</v>
+      </c>
+      <c r="F186">
+        <v>13.5419</v>
+      </c>
+      <c r="G186">
+        <v>2.605788582602575</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="1">
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <v>3000</v>
+      </c>
+      <c r="C187">
+        <v>20</v>
+      </c>
+      <c r="D187">
+        <v>7</v>
+      </c>
+      <c r="E187">
+        <v>4.096694063898378</v>
+      </c>
+      <c r="F187">
+        <v>122.3406</v>
+      </c>
+      <c r="G187">
+        <v>4.806808958167277</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" s="1">
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <v>3000</v>
+      </c>
+      <c r="C188">
+        <v>20</v>
+      </c>
+      <c r="D188">
+        <v>8</v>
+      </c>
+      <c r="E188">
+        <v>4.921172084874598</v>
+      </c>
+      <c r="F188">
+        <v>98.67489999999995</v>
+      </c>
+      <c r="G188">
+        <v>4.591830608120476</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" s="1">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>3000</v>
+      </c>
+      <c r="C189">
+        <v>20</v>
+      </c>
+      <c r="D189">
+        <v>9</v>
+      </c>
+      <c r="E189">
+        <v>6.728612806142995</v>
+      </c>
+      <c r="F189">
+        <v>14.4211</v>
+      </c>
+      <c r="G189">
+        <v>2.668692411887768</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
+      <c r="A190" s="1">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>3000</v>
+      </c>
+      <c r="C190">
+        <v>20</v>
+      </c>
+      <c r="D190">
         <v>10</v>
       </c>
-      <c r="E129">
-        <v>7.047554321581943</v>
-      </c>
-      <c r="F129">
-        <v>88.55239999999999</v>
-      </c>
-      <c r="G129">
-        <v>4.483594467193005</v>
+      <c r="E190">
+        <v>4.648590189979688</v>
+      </c>
+      <c r="F190">
+        <v>59.87579999999999</v>
+      </c>
+      <c r="G190">
+        <v>4.092272416810922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>